<commit_message>
The Crucible: Steps 8 & 9 Complete
</commit_message>
<xml_diff>
--- a/CSUN/Comp467/The Crucible/proj4_output.xlsx
+++ b/CSUN/Comp467/The Crucible/proj4_output.xlsx
@@ -122,6 +122,336 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>16</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>17</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>18</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>20</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>21</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>22</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>24</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>25</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>28</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="914400" cy="704850"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,7 +743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,6 +940,11 @@
           <t>ps_end_tc</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ps_thumb</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -628,6 +963,7 @@
           <t>00:00:05:13</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -646,6 +982,7 @@
           <t>00:00:08:23</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -664,6 +1001,7 @@
           <t>00:00:12:12</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -682,6 +1020,7 @@
           <t>00:00:16:19</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -700,6 +1039,7 @@
           <t>00:00:19:09</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -718,6 +1058,7 @@
           <t>00:00:25:14</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -736,6 +1077,7 @@
           <t>00:01:16:23</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -754,6 +1096,7 @@
           <t>00:01:33:16</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -772,6 +1115,7 @@
           <t>00:01:43:20</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -790,6 +1134,7 @@
           <t>00:01:58:23</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -808,6 +1153,7 @@
           <t>00:02:07:01</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -826,6 +1172,7 @@
           <t>00:02:24:00</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -844,8 +1191,10 @@
           <t>00:02:36:16</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>